<commit_message>
Various fixes for sensact Sattlerstraße
</commit_message>
<xml_diff>
--- a/espidf-components/sensact-applicationmodel/apps/Aufbau der Statusmeldung 4 u16.xlsx
+++ b/espidf-components/sensact-applicationmodel/apps/Aufbau der Statusmeldung 4 u16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\sensact\espidf-components\sensact-applicationmodel\apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBEFF47-6344-4035-A0FF-D193A4A555F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECEBE4F-B686-4A0C-A0A1-BFAB91973350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{461599E1-9183-4578-B934-6ADA73D392F8}"/>
   </bookViews>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>u16[0]</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Sound</t>
   </si>
   <si>
-    <t>volune</t>
-  </si>
-  <si>
     <t>melody</t>
   </si>
   <si>
@@ -269,6 +266,15 @@
   </si>
   <si>
     <t>storedLevel</t>
+  </si>
+  <si>
+    <t>muted</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>isPlaying</t>
   </si>
 </sst>
 </file>
@@ -662,7 +668,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -824,10 +830,10 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>35</v>
@@ -841,16 +847,16 @@
         <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>